<commit_message>
Added prefiltering to Project save method
</commit_message>
<xml_diff>
--- a/experiment_data/peritonitis_m_template.xlsx
+++ b/experiment_data/peritonitis_m_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t xml:space="preserve">channel</t>
   </si>
@@ -146,27 +146,138 @@
     <t xml:space="preserve">BV605\s*-*A$</t>
   </si>
   <si>
-    <t xml:space="preserve">BV711\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE\s*-*Cy\s*-*7\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmCyan\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APC\s*-*Cy\s*-*7\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*14$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*16$</t>
-  </si>
-  <si>
+    <t xml:space="preserve">.*BV711\s*-*A.*$</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PE\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PE\s*-*Cy\s*-*7\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AmCyan\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -174,17 +285,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Siglec</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">\s*-*</t>
+      <t xml:space="preserve">APC\s*-*Cy\s*-*7\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
     </r>
     <r>
       <rPr>
@@ -193,6 +303,131 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CD14 FITC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CD16 PerCP-CY5_5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Siglec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">\s*-*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">8</t>
     </r>
     <r>
@@ -201,58 +436,645 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">$</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*45$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*3$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*1\s*-*c$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*15$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA\s*-*DR$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*116$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD\s*-*19$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L\/*D$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dead,LD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSC\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSC\s*-*H$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSC\s*-*W$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSC\s*-*A$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSC\s*-*H$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSC\s*-*W$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time$</t>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Siglec8 APC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD3 APC Fire 700,CD3 APCFire750</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CD3 Fire750</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*1\s*-*c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CD1c BV421</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HLA\s*-*DR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CD\s*-*19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">L\/*D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Dead,LD,L/D-CD19-CD14,CD14_19_LD,Dead V500</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FSC\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FSC\s*-*H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FSC\s*-*W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SSC\s*-*A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SSC\s*-*H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SSC\s*-*W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -262,7 +1084,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -290,6 +1112,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -334,7 +1167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,6 +1178,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -367,10 +1208,10 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
   </cols>
@@ -525,10 +1366,10 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.34"/>
@@ -626,44 +1467,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -671,137 +1512,151 @@
       </c>
       <c r="D12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
+      <c r="B14" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>48</v>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
+      <c r="B16" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>50</v>
+      <c r="B17" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
+      <c r="B18" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>52</v>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>53</v>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>54</v>
+      <c r="B21" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>55</v>
+      <c r="B22" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>56</v>
+      <c r="B23" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>57</v>
+      <c r="D23" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>58</v>
+      <c r="B24" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
@@ -812,8 +1667,8 @@
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
+      <c r="B25" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0</v>
@@ -824,8 +1679,8 @@
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>60</v>
+      <c r="B26" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>0</v>
@@ -836,8 +1691,8 @@
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>61</v>
+      <c r="B27" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
@@ -848,8 +1703,8 @@
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>62</v>
+      <c r="B28" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>0</v>
@@ -860,8 +1715,8 @@
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
+      <c r="B29" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
@@ -872,8 +1727,8 @@
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>64</v>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added remove_file method to FCSExperiment
</commit_message>
<xml_diff>
--- a/experiment_data/peritonitis_m_template.xlsx
+++ b/experiment_data/peritonitis_m_template.xlsx
@@ -473,7 +473,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
   </cols>
@@ -628,10 +628,10 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.34"/>
@@ -774,7 +774,7 @@
       </c>
       <c r="D12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>9</v>
       </c>
@@ -788,7 +788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>11</v>
       </c>
@@ -816,7 +816,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>15</v>
       </c>

</xml_diff>